<commit_message>
added 2c and algos results
</commit_message>
<xml_diff>
--- a/Data/1500 SAs 21 Resources - For IDC.xlsx
+++ b/Data/1500 SAs 21 Resources - For IDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/304b24243408c27c/Desktop/projects/Salesforce/SalesForceProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B44550A0-81D6-4A62-9597-4B6D38B54089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B44550A0-81D6-4A62-9597-4B6D38B54089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4934949A-EFD9-4DAB-9DDC-488886FC8CC7}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1500 SAs" sheetId="1" r:id="rId1"/>
@@ -7134,13 +7134,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1501"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.77734375" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
@@ -55721,7 +55719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H1504"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tested 2 new datasets
</commit_message>
<xml_diff>
--- a/Data/1500 SAs 21 Resources - For IDC.xlsx
+++ b/Data/1500 SAs 21 Resources - For IDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/304b24243408c27c/Desktop/projects/Salesforce/SalesForceProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{B44550A0-81D6-4A62-9597-4B6D38B54089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4934949A-EFD9-4DAB-9DDC-488886FC8CC7}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{B44550A0-81D6-4A62-9597-4B6D38B54089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6E4EC09-1DEF-41F7-909A-468E51F40F7C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7134,7 +7134,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7145,6 +7147,8 @@
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>